<commit_message>
BFD done, left ooad implementation and cleaning
</commit_message>
<xml_diff>
--- a/app/bin/main/dsa/airplane_cargo.xlsx
+++ b/app/bin/main/dsa/airplane_cargo.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teoh Wei Hong\Documents\Programming\Own study\DSA\DSA\app\src\main\java\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{017FBE43-9AE6-4F56-896A-09965579B7F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD64A7FD-43C0-420A-B726-32A3AE6582AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37440" yWindow="960" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>Row No.</t>
   </si>
@@ -332,13 +332,19 @@
   </si>
   <si>
     <t>Deep-Sea Exploration Gear</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Test2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -349,10 +355,15 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -363,7 +374,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -373,27 +384,43 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -413,9 +440,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -453,7 +480,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -525,7 +552,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -546,7 +573,6 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
@@ -557,31 +583,31 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
+                <a:tint val="15000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
+                <a:tint val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
@@ -603,7 +629,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -661,7 +687,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -674,13 +700,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
+                <a:tint val="80000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -699,17 +724,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D101"/>
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="U109" sqref="U109"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -719,1404 +754,1432 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="C2" s="3">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="C3" s="3">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>10</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="D5" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6">
+      <c r="C6" s="3">
+        <v>4</v>
+      </c>
+      <c r="D6" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="C7" s="3">
+        <v>5</v>
+      </c>
+      <c r="D7" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="C8" s="3">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>10</v>
       </c>
-      <c r="D9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="D9" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>9</v>
       </c>
-      <c r="D10">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="D10" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="C11">
-        <v>4</v>
-      </c>
-      <c r="D11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="C11" s="3">
+        <v>4</v>
+      </c>
+      <c r="D11" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
       </c>
-      <c r="C12">
-        <v>5</v>
-      </c>
-      <c r="D12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="C12" s="3">
+        <v>5</v>
+      </c>
+      <c r="D12" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>15</v>
       </c>
-      <c r="C13">
-        <v>3</v>
-      </c>
-      <c r="D13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="C13" s="3">
+        <v>3</v>
+      </c>
+      <c r="D13" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
       </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14">
+      <c r="C14" s="3">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15">
+    <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>17</v>
       </c>
-      <c r="C15">
-        <v>5</v>
-      </c>
-      <c r="D15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="C15" s="3">
+        <v>5</v>
+      </c>
+      <c r="D15" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>18</v>
       </c>
-      <c r="C16">
-        <v>4</v>
-      </c>
-      <c r="D16">
+      <c r="C16" s="3">
+        <v>4</v>
+      </c>
+      <c r="D16" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17">
+    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>19</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="3">
         <v>8</v>
       </c>
-      <c r="D17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="D17" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>20</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="3">
         <v>1</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19">
+    <row r="19" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>21</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="3">
         <v>1</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20">
+    <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>22</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="3">
         <v>9</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21">
+    <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>23</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="3">
         <v>1</v>
       </c>
-      <c r="D21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22">
+      <c r="D21" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>24</v>
       </c>
-      <c r="C22">
-        <v>2</v>
-      </c>
-      <c r="D22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23">
+      <c r="C22" s="3">
+        <v>2</v>
+      </c>
+      <c r="D22" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>25</v>
       </c>
-      <c r="C23">
-        <v>4</v>
-      </c>
-      <c r="D23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24">
+      <c r="C23" s="3">
+        <v>4</v>
+      </c>
+      <c r="D23" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>26</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="3">
         <v>9</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25">
+    <row r="25" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>27</v>
       </c>
-      <c r="C25">
-        <v>5</v>
-      </c>
-      <c r="D25">
+      <c r="C25" s="3">
+        <v>5</v>
+      </c>
+      <c r="D25" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26">
+    <row r="26" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
         <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>28</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="3">
         <v>1</v>
       </c>
-      <c r="D26">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27">
+      <c r="D26" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
         <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>29</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="3">
         <v>1</v>
       </c>
-      <c r="D27">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28">
+      <c r="D27" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
         <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>30</v>
       </c>
-      <c r="C28">
-        <v>2</v>
-      </c>
-      <c r="D28">
+      <c r="C28" s="3">
+        <v>2</v>
+      </c>
+      <c r="D28" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29">
+    <row r="29" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
         <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>31</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="3">
         <v>8</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30">
+    <row r="30" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
         <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>32</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="3">
         <v>6</v>
       </c>
-      <c r="D30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31">
+      <c r="D30" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
         <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>33</v>
       </c>
-      <c r="C31">
-        <v>5</v>
-      </c>
-      <c r="D31">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32">
+      <c r="C31" s="3">
+        <v>5</v>
+      </c>
+      <c r="D31" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
         <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>34</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="3">
         <v>9</v>
       </c>
-      <c r="D32">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33">
+      <c r="D32" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
         <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>35</v>
       </c>
-      <c r="C33">
-        <v>5</v>
-      </c>
-      <c r="D33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34">
+      <c r="C33" s="3">
+        <v>5</v>
+      </c>
+      <c r="D33" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
         <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>36</v>
       </c>
-      <c r="C34">
-        <v>3</v>
-      </c>
-      <c r="D34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35">
+      <c r="C34" s="3">
+        <v>3</v>
+      </c>
+      <c r="D34" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="3">
         <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>37</v>
       </c>
-      <c r="C35">
-        <v>3</v>
-      </c>
-      <c r="D35">
+      <c r="C35" s="3">
+        <v>3</v>
+      </c>
+      <c r="D35" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36">
+    <row r="36" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="3">
         <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>38</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="3">
         <v>10</v>
       </c>
-      <c r="D36">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37">
+      <c r="D36" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="3">
         <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>39</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="3">
         <v>6</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38">
+    <row r="38" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="3">
         <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>40</v>
       </c>
-      <c r="C38">
-        <v>3</v>
-      </c>
-      <c r="D38">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39">
+      <c r="C38" s="3">
+        <v>3</v>
+      </c>
+      <c r="D38" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3">
         <v>38</v>
       </c>
       <c r="B39" t="s">
         <v>41</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="3">
         <v>8</v>
       </c>
-      <c r="D39">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40">
+      <c r="D39" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="3">
         <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>42</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="3">
         <v>10</v>
       </c>
-      <c r="D40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41">
+      <c r="D40" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="3">
         <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>43</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="3">
         <v>8</v>
       </c>
-      <c r="D41">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42">
+      <c r="D41" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="3">
         <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>44</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="3">
         <v>1</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43">
+    <row r="43" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="3">
         <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>45</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="3">
         <v>1</v>
       </c>
-      <c r="D43">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44">
+      <c r="D43" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="3">
         <v>43</v>
       </c>
       <c r="B44" t="s">
         <v>46</v>
       </c>
-      <c r="C44">
-        <v>3</v>
-      </c>
-      <c r="D44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45">
+      <c r="C44" s="3">
+        <v>3</v>
+      </c>
+      <c r="D44" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="3">
         <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>47</v>
       </c>
-      <c r="C45">
-        <v>7</v>
-      </c>
-      <c r="D45">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46">
+      <c r="C45" s="3">
+        <v>7</v>
+      </c>
+      <c r="D45" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="3">
         <v>45</v>
       </c>
       <c r="B46" t="s">
         <v>48</v>
       </c>
-      <c r="C46">
-        <v>4</v>
-      </c>
-      <c r="D46">
+      <c r="C46" s="3">
+        <v>4</v>
+      </c>
+      <c r="D46" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47">
+    <row r="47" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="3">
         <v>46</v>
       </c>
       <c r="B47" t="s">
         <v>49</v>
       </c>
-      <c r="C47">
-        <v>5</v>
-      </c>
-      <c r="D47">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48">
+      <c r="C47" s="3">
+        <v>5</v>
+      </c>
+      <c r="D47" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="3">
         <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>50</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="3">
         <v>10</v>
       </c>
-      <c r="D48">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49">
+      <c r="D48" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="3">
         <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>51</v>
       </c>
-      <c r="C49">
-        <v>4</v>
-      </c>
-      <c r="D49">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50">
+      <c r="C49" s="3">
+        <v>4</v>
+      </c>
+      <c r="D49" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="3">
         <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>52</v>
       </c>
-      <c r="C50">
-        <v>4</v>
-      </c>
-      <c r="D50">
+      <c r="C50" s="3">
+        <v>4</v>
+      </c>
+      <c r="D50" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51">
+    <row r="51" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="3">
         <v>50</v>
       </c>
       <c r="B51" t="s">
         <v>53</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="3">
         <v>9</v>
       </c>
-      <c r="D51">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52">
+      <c r="D51" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="3">
         <v>51</v>
       </c>
       <c r="B52" t="s">
         <v>54</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="3">
         <v>9</v>
       </c>
-      <c r="D52">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53">
+      <c r="D52" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="3">
         <v>52</v>
       </c>
       <c r="B53" t="s">
         <v>55</v>
       </c>
-      <c r="C53">
-        <v>4</v>
-      </c>
-      <c r="D53">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54">
+      <c r="C53" s="3">
+        <v>4</v>
+      </c>
+      <c r="D53" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="3">
         <v>53</v>
       </c>
       <c r="B54" t="s">
         <v>56</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="3">
         <v>6</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55">
+    <row r="55" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="3">
         <v>54</v>
       </c>
       <c r="B55" t="s">
         <v>57</v>
       </c>
-      <c r="C55">
-        <v>7</v>
-      </c>
-      <c r="D55">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56">
+      <c r="C55" s="3">
+        <v>7</v>
+      </c>
+      <c r="D55" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="3">
         <v>55</v>
       </c>
       <c r="B56" t="s">
         <v>58</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="3">
         <v>8</v>
       </c>
-      <c r="D56">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57">
+      <c r="D56" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="3">
         <v>56</v>
       </c>
       <c r="B57" t="s">
         <v>59</v>
       </c>
-      <c r="C57">
-        <v>2</v>
-      </c>
-      <c r="D57">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58">
+      <c r="C57" s="3">
+        <v>2</v>
+      </c>
+      <c r="D57" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="3">
         <v>57</v>
       </c>
       <c r="B58" t="s">
         <v>60</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="3">
         <v>6</v>
       </c>
-      <c r="D58">
+      <c r="D58" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59">
+    <row r="59" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="3">
         <v>58</v>
       </c>
       <c r="B59" t="s">
         <v>61</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="3">
         <v>6</v>
       </c>
-      <c r="D59">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60">
+      <c r="D59" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="3">
         <v>59</v>
       </c>
       <c r="B60" t="s">
         <v>62</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="3">
         <v>8</v>
       </c>
-      <c r="D60">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61">
+      <c r="D60" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="3">
         <v>60</v>
       </c>
       <c r="B61" t="s">
         <v>63</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="3">
         <v>6</v>
       </c>
-      <c r="D61">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62">
+      <c r="D61" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="3">
         <v>61</v>
       </c>
       <c r="B62" t="s">
         <v>64</v>
       </c>
-      <c r="C62">
+      <c r="C62" s="3">
         <v>6</v>
       </c>
-      <c r="D62">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63">
+      <c r="D62" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="3">
         <v>62</v>
       </c>
       <c r="B63" t="s">
         <v>65</v>
       </c>
-      <c r="C63">
-        <v>5</v>
-      </c>
-      <c r="D63">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64">
+      <c r="C63" s="3">
+        <v>5</v>
+      </c>
+      <c r="D63" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="3">
         <v>63</v>
       </c>
       <c r="B64" t="s">
         <v>66</v>
       </c>
-      <c r="C64">
+      <c r="C64" s="3">
         <v>10</v>
       </c>
-      <c r="D64">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65">
+      <c r="D64" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="3">
         <v>64</v>
       </c>
       <c r="B65" t="s">
         <v>67</v>
       </c>
-      <c r="C65">
-        <v>5</v>
-      </c>
-      <c r="D65">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66">
+      <c r="C65" s="3">
+        <v>5</v>
+      </c>
+      <c r="D65" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="3">
         <v>65</v>
       </c>
       <c r="B66" t="s">
         <v>68</v>
       </c>
-      <c r="C66">
-        <v>2</v>
-      </c>
-      <c r="D66">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67">
+      <c r="C66" s="3">
+        <v>2</v>
+      </c>
+      <c r="D66" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="3">
         <v>66</v>
       </c>
       <c r="B67" t="s">
         <v>69</v>
       </c>
-      <c r="C67">
+      <c r="C67" s="3">
         <v>9</v>
       </c>
-      <c r="D67">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68">
+      <c r="D67" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="3">
         <v>67</v>
       </c>
       <c r="B68" t="s">
         <v>70</v>
       </c>
-      <c r="C68">
+      <c r="C68" s="3">
         <v>9</v>
       </c>
-      <c r="D68">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69">
+      <c r="D68" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="3">
         <v>68</v>
       </c>
       <c r="B69" t="s">
         <v>71</v>
       </c>
-      <c r="C69">
-        <v>2</v>
-      </c>
-      <c r="D69">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70">
+      <c r="C69" s="3">
+        <v>2</v>
+      </c>
+      <c r="D69" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="3">
         <v>69</v>
       </c>
       <c r="B70" t="s">
         <v>72</v>
       </c>
-      <c r="C70">
-        <v>3</v>
-      </c>
-      <c r="D70">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71">
+      <c r="C70" s="3">
+        <v>3</v>
+      </c>
+      <c r="D70" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="3">
         <v>70</v>
       </c>
       <c r="B71" t="s">
         <v>73</v>
       </c>
-      <c r="C71">
-        <v>3</v>
-      </c>
-      <c r="D71">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72">
+      <c r="C71" s="3">
+        <v>3</v>
+      </c>
+      <c r="D71" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="3">
         <v>71</v>
       </c>
       <c r="B72" t="s">
         <v>74</v>
       </c>
-      <c r="C72">
-        <v>3</v>
-      </c>
-      <c r="D72">
+      <c r="C72" s="3">
+        <v>3</v>
+      </c>
+      <c r="D72" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73">
+    <row r="73" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="3">
         <v>72</v>
       </c>
       <c r="B73" t="s">
         <v>75</v>
       </c>
-      <c r="C73">
-        <v>5</v>
-      </c>
-      <c r="D73">
+      <c r="C73" s="3">
+        <v>5</v>
+      </c>
+      <c r="D73" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74">
+    <row r="74" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="3">
         <v>73</v>
       </c>
       <c r="B74" t="s">
         <v>76</v>
       </c>
-      <c r="C74">
-        <v>5</v>
-      </c>
-      <c r="D74">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75">
+      <c r="C74" s="3">
+        <v>5</v>
+      </c>
+      <c r="D74" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="3">
         <v>74</v>
       </c>
       <c r="B75" t="s">
         <v>77</v>
       </c>
-      <c r="C75">
-        <v>4</v>
-      </c>
-      <c r="D75">
+      <c r="C75" s="3">
+        <v>4</v>
+      </c>
+      <c r="D75" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76">
+    <row r="76" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="3">
         <v>75</v>
       </c>
       <c r="B76" t="s">
         <v>78</v>
       </c>
-      <c r="C76">
-        <v>4</v>
-      </c>
-      <c r="D76">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77">
+      <c r="C76" s="3">
+        <v>4</v>
+      </c>
+      <c r="D76" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="3">
         <v>76</v>
       </c>
       <c r="B77" t="s">
         <v>79</v>
       </c>
-      <c r="C77">
+      <c r="C77" s="3">
         <v>8</v>
       </c>
-      <c r="D77">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78">
+      <c r="D77" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="3">
         <v>77</v>
       </c>
       <c r="B78" t="s">
         <v>80</v>
       </c>
-      <c r="C78">
-        <v>2</v>
-      </c>
-      <c r="D78">
+      <c r="C78" s="3">
+        <v>2</v>
+      </c>
+      <c r="D78" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79">
+    <row r="79" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="3">
         <v>78</v>
       </c>
       <c r="B79" t="s">
         <v>81</v>
       </c>
-      <c r="C79">
+      <c r="C79" s="3">
         <v>8</v>
       </c>
-      <c r="D79">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80">
+      <c r="D79" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="3">
         <v>79</v>
       </c>
       <c r="B80" t="s">
         <v>82</v>
       </c>
-      <c r="C80">
-        <v>5</v>
-      </c>
-      <c r="D80">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81">
+      <c r="C80" s="3">
+        <v>5</v>
+      </c>
+      <c r="D80" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="3">
         <v>80</v>
       </c>
       <c r="B81" t="s">
         <v>83</v>
       </c>
-      <c r="C81">
+      <c r="C81" s="3">
         <v>6</v>
       </c>
-      <c r="D81">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82">
+      <c r="D81" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="3">
         <v>81</v>
       </c>
       <c r="B82" t="s">
         <v>84</v>
       </c>
-      <c r="C82">
+      <c r="C82" s="3">
         <v>9</v>
       </c>
-      <c r="D82">
+      <c r="D82" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83">
+    <row r="83" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="3">
         <v>82</v>
       </c>
       <c r="B83" t="s">
         <v>85</v>
       </c>
-      <c r="C83">
+      <c r="C83" s="3">
         <v>8</v>
       </c>
-      <c r="D83">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84">
+      <c r="D83" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="3">
         <v>83</v>
       </c>
       <c r="B84" t="s">
         <v>86</v>
       </c>
-      <c r="C84">
+      <c r="C84" s="3">
         <v>6</v>
       </c>
-      <c r="D84">
+      <c r="D84" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85">
+    <row r="85" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="3">
         <v>84</v>
       </c>
       <c r="B85" t="s">
         <v>87</v>
       </c>
-      <c r="C85">
-        <v>7</v>
-      </c>
-      <c r="D85">
+      <c r="C85" s="3">
+        <v>7</v>
+      </c>
+      <c r="D85" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86">
+    <row r="86" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="3">
         <v>85</v>
       </c>
       <c r="B86" t="s">
         <v>88</v>
       </c>
-      <c r="C86">
+      <c r="C86" s="3">
         <v>8</v>
       </c>
-      <c r="D86">
+      <c r="D86" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87">
+    <row r="87" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="3">
         <v>86</v>
       </c>
       <c r="B87" t="s">
         <v>89</v>
       </c>
-      <c r="C87">
-        <v>3</v>
-      </c>
-      <c r="D87">
+      <c r="C87" s="3">
+        <v>3</v>
+      </c>
+      <c r="D87" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88">
+    <row r="88" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="3">
         <v>87</v>
       </c>
       <c r="B88" t="s">
         <v>90</v>
       </c>
-      <c r="C88">
+      <c r="C88" s="3">
         <v>9</v>
       </c>
-      <c r="D88">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89">
+      <c r="D88" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="3">
         <v>88</v>
       </c>
       <c r="B89" t="s">
         <v>91</v>
       </c>
-      <c r="C89">
+      <c r="C89" s="3">
         <v>1</v>
       </c>
-      <c r="D89">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90">
+      <c r="D89" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="3">
         <v>89</v>
       </c>
       <c r="B90" t="s">
         <v>92</v>
       </c>
-      <c r="C90">
+      <c r="C90" s="3">
         <v>8</v>
       </c>
-      <c r="D90">
+      <c r="D90" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91">
+    <row r="91" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="3">
         <v>90</v>
       </c>
       <c r="B91" t="s">
         <v>93</v>
       </c>
-      <c r="C91">
-        <v>7</v>
-      </c>
-      <c r="D91">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92">
+      <c r="C91" s="3">
+        <v>7</v>
+      </c>
+      <c r="D91" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="3">
         <v>91</v>
       </c>
       <c r="B92" t="s">
         <v>94</v>
       </c>
-      <c r="C92">
+      <c r="C92" s="3">
         <v>6</v>
       </c>
-      <c r="D92">
+      <c r="D92" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93">
+    <row r="93" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="3">
         <v>92</v>
       </c>
       <c r="B93" t="s">
         <v>95</v>
       </c>
-      <c r="C93">
+      <c r="C93" s="3">
         <v>6</v>
       </c>
-      <c r="D93">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94">
+      <c r="D93" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="3">
         <v>93</v>
       </c>
       <c r="B94" t="s">
         <v>96</v>
       </c>
-      <c r="C94">
-        <v>4</v>
-      </c>
-      <c r="D94">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95">
+      <c r="C94" s="3">
+        <v>4</v>
+      </c>
+      <c r="D94" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="3">
         <v>94</v>
       </c>
       <c r="B95" t="s">
         <v>97</v>
       </c>
-      <c r="C95">
-        <v>7</v>
-      </c>
-      <c r="D95">
+      <c r="C95" s="3">
+        <v>7</v>
+      </c>
+      <c r="D95" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96">
+    <row r="96" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="3">
         <v>95</v>
       </c>
       <c r="B96" t="s">
         <v>98</v>
       </c>
-      <c r="C96">
+      <c r="C96" s="3">
         <v>9</v>
       </c>
-      <c r="D96">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97">
+      <c r="D96" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="3">
         <v>96</v>
       </c>
       <c r="B97" t="s">
         <v>99</v>
       </c>
-      <c r="C97">
+      <c r="C97" s="3">
         <v>8</v>
       </c>
-      <c r="D97">
+      <c r="D97" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98">
+    <row r="98" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="3">
         <v>97</v>
       </c>
       <c r="B98" t="s">
         <v>100</v>
       </c>
-      <c r="C98">
-        <v>5</v>
-      </c>
-      <c r="D98">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A99">
+      <c r="C98" s="3">
+        <v>5</v>
+      </c>
+      <c r="D98" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="3">
         <v>98</v>
       </c>
       <c r="B99" t="s">
         <v>101</v>
       </c>
-      <c r="C99">
-        <v>5</v>
-      </c>
-      <c r="D99">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A100">
+      <c r="C99" s="3">
+        <v>5</v>
+      </c>
+      <c r="D99" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="3">
         <v>99</v>
       </c>
       <c r="B100" t="s">
         <v>102</v>
       </c>
-      <c r="C100">
-        <v>4</v>
-      </c>
-      <c r="D100">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A101">
+      <c r="C100" s="3">
+        <v>4</v>
+      </c>
+      <c r="D100" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="3">
         <v>100</v>
       </c>
       <c r="B101" t="s">
         <v>103</v>
       </c>
-      <c r="C101">
-        <v>5</v>
-      </c>
-      <c r="D101">
-        <v>2</v>
+      <c r="C101" s="3">
+        <v>5</v>
+      </c>
+      <c r="D101" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" s="4">
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
+        <v>104</v>
+      </c>
+      <c r="C102" s="4">
+        <v>10</v>
+      </c>
+      <c r="D102" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" s="4">
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
+        <v>105</v>
+      </c>
+      <c r="C103" s="4">
+        <v>9</v>
+      </c>
+      <c r="D103" s="4">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>